<commit_message>
Added test cases in Ninja_Isango_Test_Cases.xlsx
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="2" r:id="rId1"/>
     <sheet name="Home Page" sheetId="4" r:id="rId2"/>
     <sheet name="Search" sheetId="5" r:id="rId3"/>
+    <sheet name="Product Deatil Page" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="163">
   <si>
     <t>Project Name:</t>
   </si>
@@ -625,6 +627,41 @@
   </si>
   <si>
     <t>Application display search results as per search term.</t>
+  </si>
+  <si>
+    <t>Verify application displays product detail page when user click on product display on home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch Ninja specific URL.
+2. User is on Home Page
+3. Perform search and click on product display as search result.
+</t>
+  </si>
+  <si>
+    <t>Verify application displays product detail page when user click on product display as search result.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch Ninja specific URL.
+2. User is on Home Page
+3. Click on product.
+4. User is on product detail page.
+</t>
+  </si>
+  <si>
+    <t>Verify application allow user to perform search from search module display on search result page.</t>
+  </si>
+  <si>
+    <t>Verify application displays  search result page when user click on "
+Show all tours and activities"</t>
+  </si>
+  <si>
+    <t>Verify application displays product image in frame and allow user to flash other available images.</t>
+  </si>
+  <si>
+    <t>Application allow user to change image using next and previous button. Also user can change image using click on image icons.</t>
+  </si>
+  <si>
+    <t>Verify application displays header and footer on product detail page.</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1347,6 +1384,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1390,6 +1430,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1446,24 +1504,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1476,6 +1516,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1990,6 +2033,251 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2255,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,20 +2557,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="56"/>
+      <c r="A1" s="56"/>
+      <c r="B1" s="57"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="59"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="59"/>
-      <c r="B4" s="60"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="61"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2394,14 +2682,14 @@
       <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -2447,85 +2735,85 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="64"/>
+      <c r="C22" s="65"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="53">
+      <c r="B23" s="54">
         <f>COUNTIF('Home Page'!A17:A142,"*")</f>
         <v>21</v>
       </c>
-      <c r="C23" s="54"/>
+      <c r="C23" s="55"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="53">
+      <c r="B24" s="54">
         <f>COUNTIF(Search!A17:A132,"*")</f>
         <v>25</v>
       </c>
-      <c r="C24" s="54"/>
+      <c r="C24" s="55"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="54"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="54"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="55"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="53"/>
-      <c r="C27" s="54"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="55"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="54"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="55"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="54"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="65">
+      <c r="B30" s="66">
         <f>SUM(B23:B29)</f>
         <v>46</v>
       </c>
-      <c r="C30" s="66"/>
+      <c r="C30" s="67"/>
     </row>
     <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2576,15 +2864,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
@@ -2592,29 +2880,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="87"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="69"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90"/>
-      <c r="B4" s="91"/>
-    </row>
-    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
       <c r="C5" s="48"/>
       <c r="D5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="82" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -2627,7 +2915,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
+      <c r="A7" s="83"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -2637,12 +2925,12 @@
       </c>
       <c r="D7" s="25"/>
     </row>
-    <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="84"/>
+      <c r="B8" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -2653,11 +2941,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="82"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G61,"PENDING")</f>
         <v>0</v>
@@ -2668,11 +2956,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="92"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G61,"IN PROGRESS")</f>
         <v>0</v>
@@ -2683,11 +2971,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="85"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G61,"BLOCKED")</f>
         <v>0</v>
@@ -2698,28 +2986,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="70">
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="77">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="77">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -2751,7 +3039,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>90</v>
       </c>
@@ -2800,7 +3088,7 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
     </row>
-    <row r="20" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>93</v>
       </c>
@@ -2932,7 +3220,7 @@
       <c r="F27" s="28"/>
       <c r="G27" s="28"/>
     </row>
-    <row r="28" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="300" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>101</v>
       </c>
@@ -2947,7 +3235,7 @@
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
     </row>
-    <row r="29" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>102</v>
       </c>
@@ -3131,8 +3419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3147,27 +3435,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86"/>
-      <c r="B1" s="87"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="69"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="90"/>
-      <c r="B4" s="91"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="82" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -3180,7 +3468,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
+      <c r="A7" s="83"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -3191,11 +3479,11 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
-      <c r="B8" s="78" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -3206,11 +3494,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="81"/>
-      <c r="C9" s="82"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G49,"PENDING")</f>
         <v>0</v>
@@ -3221,11 +3509,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83" t="s">
+      <c r="A10" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="92"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G49,"IN PROGRESS")</f>
         <v>0</v>
@@ -3236,11 +3524,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="85"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G49,"BLOCKED")</f>
         <v>0</v>
@@ -3251,28 +3539,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="68"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="70">
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="77">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="70">
+      <c r="E12" s="77">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -3304,7 +3592,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>90</v>
       </c>
@@ -3342,7 +3630,7 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
     </row>
-    <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>92</v>
       </c>
@@ -3408,7 +3696,7 @@
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
     </row>
-    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>96</v>
       </c>
@@ -3474,7 +3762,7 @@
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
     </row>
-    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>100</v>
       </c>
@@ -3492,14 +3780,14 @@
       <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="93" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="93"/>
-      <c r="D28" s="93"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="94"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
     </row>
     <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
@@ -3570,14 +3858,14 @@
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="94"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="95"/>
     </row>
     <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
@@ -3772,4 +4060,299 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="68"/>
+      <c r="B1" s="69"/>
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
+    </row>
+    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
+    </row>
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="21">
+        <f>COUNTIF(F17:F49,"PASSED")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="83"/>
+      <c r="B7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="24">
+        <f>COUNTIF(F17:F49,"FAILED")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="84"/>
+      <c r="B8" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="86"/>
+      <c r="D8" s="43">
+        <f>SUM(C6,C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <f>SUM(D6,D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="87" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="44">
+        <f>COUNTIF(G17:G49,"PENDING")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="45">
+        <f>COUNTIF(F17:F49,"PENDING")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="91"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="45">
+        <f>COUNTIF(G17:G49,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="45">
+        <f>COUNTIF(F17:F49,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="91"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="45">
+        <f>COUNTIF(G17:G49,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="45">
+        <f>COUNTIF(F17:F49,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="77">
+        <f>SUM(D8:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="77">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="80"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="16" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="96" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="96" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C22" s="96" t="s">
+        <v>162</v>
+      </c>
+      <c r="E22" s="96"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="96"/>
+      <c r="E23" s="96"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="96"/>
+      <c r="E24" s="96"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="96"/>
+      <c r="E25" s="96"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="96"/>
+      <c r="E26" s="96"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="96"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="96"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="96"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="96"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="96"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test cases for product detail page in Ninja_Isango_Test_Cases.xlsx
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -16,9 +16,9 @@
     <sheet name="Home Page" sheetId="4" r:id="rId2"/>
     <sheet name="Search" sheetId="5" r:id="rId3"/>
     <sheet name="Product Deatil Page" sheetId="6" r:id="rId4"/>
+    <sheet name="Availability Page" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="184">
   <si>
     <t>Project Name:</t>
   </si>
@@ -662,6 +662,104 @@
   </si>
   <si>
     <t>Verify application displays header and footer on product detail page.</t>
+  </si>
+  <si>
+    <t>Verify number of child age dropdown down as per value selected in children drop down.</t>
+  </si>
+  <si>
+    <t>Verify application display below mentioned sections in product description:
+1. Why book this tour
+2. Customer reviews 
+3. Tour information
+4. Activity schedule
+5. Itinerary
+6. Inclusions and Exclusions
+7. cancellation policy
+8. You may also be interested in</t>
+  </si>
+  <si>
+    <t>Verify application allow user to change currency from dropdown display in footer.</t>
+  </si>
+  <si>
+    <t>Application fix this currency change through out the session.</t>
+  </si>
+  <si>
+    <t>Verify application display below mentioned information with all item display under heading "You may also be interested in"
+1. Product Image
+2. Star rating
+3. Product Name
+4. Product description
+5. Book Now button
+6. Product Price</t>
+  </si>
+  <si>
+    <t>Verify application allow user to share product details on social media using social media icons display on product detail page.</t>
+  </si>
+  <si>
+    <t>Application allow user to share and verify shared content on social media.</t>
+  </si>
+  <si>
+    <t>Application display cross button also associated with pane to close the same.</t>
+  </si>
+  <si>
+    <t>Verify application displays map when user click on link "See on map"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Launch Ninja specific URL.
+2. User is on Home Page
+3. Click on product.
+4. User is on product detail page.
+5. Add product in cart
+6. Navigate to product detail page.
+</t>
+  </si>
+  <si>
+    <t>Verify application flash cart information when user perform mouse hover on cart link display on top right corner.</t>
+  </si>
+  <si>
+    <t>Application display cart information with Go to cart button.</t>
+  </si>
+  <si>
+    <t>Verify application navigate user when click on Go to cart button display on mouse hover on cart link</t>
+  </si>
+  <si>
+    <t>Application display consistent added products and price.</t>
+  </si>
+  <si>
+    <t>1. Launch Ninja specific URL.
+2. User is on Home Page
+3. Click on product.
+4. User is on product detail page.
+5. Enter valid information and click on Check availability button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify application displays </t>
+  </si>
+  <si>
+    <t>Verify application displays below mentioned fields:
+1. Product name
+2. Social Icons
+3. Star rating 
+4. Lowest Price guaranteed logo
+5. Product Image</t>
+  </si>
+  <si>
+    <t>Verify application display availability module with below mentioned information:
+1. Product Price
+2. Travel Date (Date / Month Year)
+3. Check Availability
+4. Adult dropdown
+5. Children dropdown
+6. Child policy (IF applicable)</t>
+  </si>
+  <si>
+    <t>Application display product detail page when user click on product display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify application display "Cancellation policy" in floating pane when user click on Cancellation policy link. </t>
+  </si>
+  <si>
+    <t>Application displays map in floating pane with close button.</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1384,8 +1482,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1424,12 +1525,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1516,9 +1611,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2278,6 +2370,251 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2543,8 +2880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,20 +2894,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57"/>
+      <c r="A1" s="57"/>
+      <c r="B1" s="58"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="60"/>
-      <c r="B4" s="61"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="62"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2682,14 +3019,14 @@
       <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62" t="s">
+      <c r="A16" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -2735,85 +3072,88 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="65"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="66"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="65"/>
+      <c r="C22" s="66"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="54">
+      <c r="B23" s="55">
         <f>COUNTIF('Home Page'!A17:A142,"*")</f>
         <v>21</v>
       </c>
-      <c r="C23" s="55"/>
+      <c r="C23" s="56"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="54">
+      <c r="B24" s="55">
         <f>COUNTIF(Search!A17:A132,"*")</f>
         <v>25</v>
       </c>
-      <c r="C24" s="55"/>
+      <c r="C24" s="56"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="55"/>
+      <c r="B25" s="55">
+        <f>COUNTIF('Product Deatil Page'!A17:A39,"*")</f>
+        <v>17</v>
+      </c>
+      <c r="C25" s="56"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="55"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="56"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="55"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="55"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="55"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="66">
+      <c r="B30" s="53">
         <f>SUM(B23:B29)</f>
-        <v>46</v>
-      </c>
-      <c r="C30" s="67"/>
+        <v>63</v>
+      </c>
+      <c r="C30" s="54"/>
     </row>
     <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2842,18 +3182,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A1:B4"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2880,20 +3220,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
-      <c r="B1" s="69"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="68"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="71"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="71"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="73"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
@@ -2902,7 +3242,7 @@
       <c r="D5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="81" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -2915,7 +3255,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -2926,11 +3266,11 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -2941,11 +3281,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="89"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G61,"PENDING")</f>
         <v>0</v>
@@ -2956,11 +3296,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G61,"IN PROGRESS")</f>
         <v>0</v>
@@ -2971,11 +3311,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G61,"BLOCKED")</f>
         <v>0</v>
@@ -2986,28 +3326,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="77">
+      <c r="B12" s="74"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="76">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="77">
+      <c r="E12" s="76">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -3419,7 +3759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -3435,27 +3775,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
-      <c r="B1" s="69"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="68"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="71"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="71"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="73"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="81" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -3468,7 +3808,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -3479,11 +3819,11 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -3494,11 +3834,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="89"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G49,"PENDING")</f>
         <v>0</v>
@@ -3509,11 +3849,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G49,"IN PROGRESS")</f>
         <v>0</v>
@@ -3524,11 +3864,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G49,"BLOCKED")</f>
         <v>0</v>
@@ -3539,28 +3879,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="77">
+      <c r="B12" s="74"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="76">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="77">
+      <c r="E12" s="76">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -3780,14 +4120,14 @@
       <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="93" t="s">
+      <c r="B28" s="92" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="95"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="94"/>
     </row>
     <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
@@ -3858,14 +4198,14 @@
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="93" t="s">
+      <c r="B33" s="92" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="94"/>
-      <c r="G33" s="95"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="94"/>
     </row>
     <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
@@ -4064,10 +4404,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4077,60 +4417,60 @@
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68"/>
-      <c r="B1" s="69"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="68"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="71"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="71"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72"/>
-      <c r="B4" s="73"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="81" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="21">
-        <f>COUNTIF(F17:F49,"PASSED")</f>
+        <f>COUNTIF(F17:F46,"PASSED")</f>
         <v>0</v>
       </c>
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="24">
-        <f>COUNTIF(F17:F49,"FAILED")</f>
+        <f>COUNTIF(F17:F46,"FAILED")</f>
         <v>0</v>
       </c>
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="86"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -4141,73 +4481,73 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="89"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="44">
-        <f>COUNTIF(G17:G49,"PENDING")</f>
+        <f>COUNTIF(G17:G46,"PENDING")</f>
         <v>0</v>
       </c>
       <c r="E9" s="45">
-        <f>COUNTIF(F17:F49,"PENDING")</f>
+        <f>COUNTIF(F17:F46,"PENDING")</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="92"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="91"/>
       <c r="D10" s="45">
-        <f>COUNTIF(G17:G49,"IN PROGRESS")</f>
+        <f>COUNTIF(G17:G46,"IN PROGRESS")</f>
         <v>0</v>
       </c>
       <c r="E10" s="45">
-        <f>COUNTIF(F17:F49,"IN PROGRESS")</f>
+        <f>COUNTIF(F17:F46,"IN PROGRESS")</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="45">
-        <f>COUNTIF(G17:G49,"BLOCKED")</f>
+        <f>COUNTIF(G17:G46,"BLOCKED")</f>
         <v>0</v>
       </c>
       <c r="E11" s="45">
-        <f>COUNTIF(F17:F49,"BLOCKED")</f>
+        <f>COUNTIF(F17:F46,"BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="77">
+      <c r="B12" s="74"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="76">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="77">
+      <c r="E12" s="76">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="78"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -4276,9 +4616,13 @@
       <c r="B19" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="29" t="s">
         <v>158</v>
       </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
@@ -4287,57 +4631,433 @@
       <c r="B20" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="96" t="s">
+      <c r="C20" s="52" t="s">
         <v>159</v>
       </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>94</v>
+      </c>
       <c r="B21" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="52" t="s">
         <v>160</v>
       </c>
-      <c r="E21" s="96" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="52" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C22" s="96" t="s">
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C22" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="96"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="96"/>
-      <c r="E23" s="96"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="96"/>
-      <c r="E24" s="96"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="96"/>
-      <c r="E25" s="96"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="96"/>
-      <c r="E26" s="96"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="96"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="96"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="96"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="96"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="96"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="28"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+    </row>
+    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="52" t="s">
+        <v>166</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+    </row>
+    <row r="30" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="28"/>
+      <c r="E31" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+    </row>
+    <row r="32" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+    </row>
+    <row r="33" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="67"/>
+      <c r="B1" s="68"/>
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+    </row>
+    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
+    </row>
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71"/>
+      <c r="B4" s="72"/>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="21">
+        <f>COUNTIF(F17:F46,"PASSED")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="82"/>
+      <c r="B7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="24">
+        <f>COUNTIF(F17:F46,"FAILED")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="83"/>
+      <c r="B8" s="84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="85"/>
+      <c r="D8" s="43">
+        <f>SUM(C6,C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <f>SUM(D6,D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="87"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="44">
+        <f>COUNTIF(G17:G46,"PENDING")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="45">
+        <f>COUNTIF(F17:F46,"PENDING")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="90"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="45">
+        <f>COUNTIF(G17:G46,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="45">
+        <f>COUNTIF(F17:F46,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="90"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="45">
+        <f>COUNTIF(G17:G46,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="45">
+        <f>COUNTIF(F17:F46,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="74"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="76">
+        <f>SUM(D8:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="76">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="16" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Added Cart Page test cases in Ninja_Isango_Test_Cases.xlsx
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="2" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="Search" sheetId="5" r:id="rId3"/>
     <sheet name="Product Deatil Page" sheetId="6" r:id="rId4"/>
     <sheet name="Availability Page" sheetId="7" r:id="rId5"/>
+    <sheet name="Cart Page" sheetId="8" r:id="rId6"/>
+    <sheet name="Checkout" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="259">
   <si>
     <t>Project Name:</t>
   </si>
@@ -873,6 +875,224 @@
   </si>
   <si>
     <t>Verify application substract discount cost and diplay total cost on avilibility page.</t>
+  </si>
+  <si>
+    <t>Verify application display cart page.</t>
+  </si>
+  <si>
+    <t>Application displays products added by customer.</t>
+  </si>
+  <si>
+    <t>Verify application display header and footer on cart page.</t>
+  </si>
+  <si>
+    <t>Verify items display on cart page with product added in cart.
+1. Product Name
+2. Product description
+3. Key facts
+4. Total product cost
+5. Change date/ number of travellers
+6. View price guide
+7. Remove
+8. Price per person
+9. Who's going
+10. When you're going</t>
+  </si>
+  <si>
+    <t>Verify application navigate user to product detail page for same product.</t>
+  </si>
+  <si>
+    <t>1. Launch Ninja specific URL.
+2. User is on Home Page
+3. Click on product that have options.
+4. User is on product detail page.
+5. Enter valid information and click on Check availability button
+6. User is on availability page and click on add to cart.</t>
+  </si>
+  <si>
+    <t>All links working as expected in both header and footer.</t>
+  </si>
+  <si>
+    <t>Application display all these fields for all products added in cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. click on Change date/ number of travellers button.
+</t>
+  </si>
+  <si>
+    <t>Application display same information in availability module as entered by user while adding the product into cart.</t>
+  </si>
+  <si>
+    <t>Verify application allow user to change travel date/ number of travellers on product detail page and check availability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Add another product.
+3. User is in cart page.
+</t>
+  </si>
+  <si>
+    <t>Verify application added items in cart in queue fashion.</t>
+  </si>
+  <si>
+    <t>Verify application displays Confirmation alert box with message "Are you sure you want to delete &lt;&lt;Product Name&gt;&gt; from your cart?", with "Yes" and "NO" button</t>
+  </si>
+  <si>
+    <t>Application remove product when user click on yes button and do nothing when click on NO button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Add 2 another products in cart.
+3. User is in cart page.
+4. Click on remove associated with product in cart.
+</t>
+  </si>
+  <si>
+    <t>Application update the Total Price on cart page as per remaining products in cart.</t>
+  </si>
+  <si>
+    <t>Verify application apply multisave discount on each product added starting from second product onwards.</t>
+  </si>
+  <si>
+    <t>Application apply multisave discount on all products added in cart, except first product added.</t>
+  </si>
+  <si>
+    <t>Application maintain queue while delete product from cart and product on the front not with discount.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Add 2 another products in cart.
+3. User is in cart page.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Add 2 another products in cart.
+3. User is in cart page.
+4. Click on remove link.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Add 2 another products in cart.
+3. User is in cart page.
+4. Click on Continue shopping button.
+</t>
+  </si>
+  <si>
+    <t>Verify application navigate user on home page when user click on 
+Continue shopping button.</t>
+  </si>
+  <si>
+    <t>Verify application displays message "There are no items in your travel cart. Click on "Continue Shopping" to resume your shopping." when user remove all products from cart using remove link.</t>
+  </si>
+  <si>
+    <t>Verify application displays cross sell module.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+</t>
+  </si>
+  <si>
+    <t>Verify application display "lowest price guarantee" logo.</t>
+  </si>
+  <si>
+    <t>Verify application display "Secure Checkout" button</t>
+  </si>
+  <si>
+    <t>Verify application displays Checkout page when user click on "Secure Checkout" button</t>
+  </si>
+  <si>
+    <t>1. User is on availability page and click on add to cart.
+2. Click on "Secure Checkout" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Click on book now button display with products display under cross selling module
+</t>
+  </si>
+  <si>
+    <t>Verify application remove relative product from cart.</t>
+  </si>
+  <si>
+    <t>Verify application remove product and adjust remaining products multisave accordingly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Add 2 another products in cart.
+3. User is in cart page.
+4. Remove all products using Remove link associated with products on cart page.
+</t>
+  </si>
+  <si>
+    <t>Verify application display below mentioned item with each product display on cross sell module:
+1. Heading "Book additional activities and get 5%off! We recommend..."
+2. Product Image
+3. Star rating
+4. Product Name
+5. Product description
+6. Regular price 
+7. Discounted price (Multisave options)</t>
+  </si>
+  <si>
+    <t>Verify application display product detail page.</t>
+  </si>
+  <si>
+    <t>Verify for all book now buttons application navigated to product detail page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+</t>
+  </si>
+  <si>
+    <t>Verify applicationn displays "Do you have a gift voucher/discount code?"</t>
+  </si>
+  <si>
+    <t>Verify application display text box when user click on "Do you have a gift voucher/discount code?" and display below mentioned items:
+1. Text Label "Enter your voucher/discount code."
+2. Link "Apply discount"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Click on "Do you have a gift voucher/discount code?"
+</t>
+  </si>
+  <si>
+    <t>Verify application displays below mentioned message when user enter invalid coupan:
+"The Gift Voucher / Promotional Code is either invalid or has already been consumed"</t>
+  </si>
+  <si>
+    <t>1. User is on availability page and click on add to cart.
+2. Click on "Do you have a gift voucher/discount code?"
+3. Enter invlaid code 
+4. Click on "Apply discount"</t>
+  </si>
+  <si>
+    <t>Verify application displays Text "Click CHECKOUT to complete traveller details and pay."</t>
+  </si>
+  <si>
+    <t>Verify application display "Checkout" page when user click on CHECKOUT link.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on availability page and click on add to cart.
+2. Click on CHECKOUT link.
+</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>1. Launch Ninja specific URL.
+2. User is on Home Page
+3. Click on product that have options.
+4. User is on product detail page.
+5. Enter valid information and click on Check availability button
+6. User is on availability page and click on add to cart.
+7. User is on Cart page and click on secure checkout</t>
+  </si>
+  <si>
+    <t>Verify application display Checkout page.</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1595,11 +1815,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1638,6 +1871,12 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1725,24 +1964,8 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2747,6 +2970,496 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3010,10 +3723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C27"/>
+      <selection activeCell="B28" sqref="B28:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3026,20 +3739,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-      <c r="B1" s="58"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3151,14 +3864,14 @@
       <c r="F15" s="31"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -3204,131 +3917,142 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="65"/>
-      <c r="C21" s="66"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="66"/>
+      <c r="C22" s="70"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="55">
+      <c r="B23" s="59">
         <f>COUNTIF('Home Page'!A17:A142,"*")</f>
         <v>21</v>
       </c>
-      <c r="C23" s="56"/>
+      <c r="C23" s="60"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="55">
+      <c r="B24" s="59">
         <f>COUNTIF(Search!A17:A132,"*")</f>
         <v>25</v>
       </c>
-      <c r="C24" s="56"/>
+      <c r="C24" s="60"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="55">
+      <c r="B25" s="59">
         <f>COUNTIF('Product Deatil Page'!A17:A39,"*")</f>
         <v>17</v>
       </c>
-      <c r="C25" s="56"/>
+      <c r="C25" s="60"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="55">
+      <c r="B26" s="59">
         <f>COUNTIF('Availability Page'!A17:A30,"*")</f>
         <v>14</v>
       </c>
-      <c r="C26" s="56"/>
+      <c r="C26" s="60"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="56"/>
+      <c r="B27" s="59">
+        <f>COUNTIF('Cart Page'!A17:A70,"*")</f>
+        <v>23</v>
+      </c>
+      <c r="C27" s="60"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" s="59"/>
+      <c r="C28" s="60"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="56"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39" t="s">
+      <c r="B29" s="59"/>
+      <c r="C29" s="60"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="56"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40" t="s">
+      <c r="B30" s="59"/>
+      <c r="C30" s="60"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="53">
-        <f>SUM(B23:B29)</f>
-        <v>77</v>
-      </c>
-      <c r="C30" s="54"/>
-    </row>
-    <row r="38" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>16</v>
-      </c>
+      <c r="B31" s="71">
+        <f>SUM(B23:B30)</f>
+        <v>100</v>
+      </c>
+      <c r="C31" s="72"/>
     </row>
     <row r="39" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3355,20 +4079,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67"/>
-      <c r="B1" s="68"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
@@ -3377,7 +4101,7 @@
       <c r="D5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -3390,7 +4114,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -3401,11 +4125,11 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84" t="s">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="85"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -3416,11 +4140,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G61,"PENDING")</f>
         <v>0</v>
@@ -3431,11 +4155,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G61,"IN PROGRESS")</f>
         <v>0</v>
@@ -3446,11 +4170,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G61,"BLOCKED")</f>
         <v>0</v>
@@ -3461,28 +4185,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76">
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="82">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -3880,7 +4604,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Cover Page'!$A$38:$A$42</xm:f>
+            <xm:f>'Cover Page'!$A$39:$A$43</xm:f>
           </x14:formula1>
           <xm:sqref>F17:F37</xm:sqref>
         </x14:dataValidation>
@@ -3910,27 +4634,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67"/>
-      <c r="B1" s="68"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -3943,7 +4667,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -3954,11 +4678,11 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84" t="s">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="85"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -3969,11 +4693,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G49,"PENDING")</f>
         <v>0</v>
@@ -3984,11 +4708,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G49,"IN PROGRESS")</f>
         <v>0</v>
@@ -3999,11 +4723,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G49,"BLOCKED")</f>
         <v>0</v>
@@ -4014,28 +4738,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76">
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="82">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -4255,14 +4979,14 @@
       <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="98" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="93"/>
-      <c r="D28" s="93"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="94"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="100"/>
     </row>
     <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
@@ -4333,14 +5057,14 @@
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="98" t="s">
         <v>148</v>
       </c>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="94"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="100"/>
     </row>
     <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
@@ -4519,6 +5243,14 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="B28:G28"/>
   </mergeCells>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F29:F32">
+      <formula1>$A$39:$A$43</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34:F42">
+      <formula1>$A$39:$A$43</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4527,9 +5259,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Cover Page'!$A$38:$A$42</xm:f>
+            <xm:f>'Cover Page'!$A$39:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>F17:F27 F29:F32 F34:F42</xm:sqref>
+          <xm:sqref>F17:F27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4541,7 +5273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -4557,27 +5289,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67"/>
-      <c r="B1" s="68"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -4590,7 +5322,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -4601,11 +5333,11 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84" t="s">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="85"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -4616,11 +5348,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G46,"PENDING")</f>
         <v>0</v>
@@ -4631,11 +5363,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G46,"IN PROGRESS")</f>
         <v>0</v>
@@ -4646,11 +5378,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G46,"BLOCKED")</f>
         <v>0</v>
@@ -4661,28 +5393,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76">
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="82">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -5007,8 +5739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD59"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5023,27 +5755,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67"/>
-      <c r="B1" s="68"/>
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
     </row>
     <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69"/>
-      <c r="B3" s="70"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="72"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
     </row>
     <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -5056,7 +5788,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="82"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="23" t="s">
         <v>17</v>
       </c>
@@ -5067,11 +5799,11 @@
       <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84" t="s">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="85"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="43">
         <f>SUM(C6,C7)</f>
         <v>0</v>
@@ -5082,11 +5814,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
       <c r="D9" s="44">
         <f>COUNTIF(G17:G30,"PENDING")</f>
         <v>0</v>
@@ -5097,11 +5829,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
+      <c r="A10" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
       <c r="D10" s="45">
         <f>COUNTIF(G17:G30,"IN PROGRESS")</f>
         <v>0</v>
@@ -5112,11 +5844,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="45">
         <f>COUNTIF(G17:G30,"BLOCKED")</f>
         <v>0</v>
@@ -5127,28 +5859,28 @@
       </c>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76">
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82">
         <f>SUM(D8:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="76">
+      <c r="E12" s="82">
         <f>SUM(E8:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="79"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41"/>
@@ -5180,8 +5912,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="96" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="95" t="s">
+    <row r="17" spans="1:7" s="54" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
         <v>90</v>
       </c>
       <c r="B17" s="19" t="s">
@@ -5197,8 +5929,8 @@
       <c r="F17" s="51"/>
       <c r="G17" s="51"/>
     </row>
-    <row r="18" spans="1:7" s="96" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A18" s="95" t="s">
+    <row r="18" spans="1:7" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="53" t="s">
         <v>91</v>
       </c>
       <c r="B18" s="19" t="s">
@@ -5214,8 +5946,8 @@
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
     </row>
-    <row r="19" spans="1:7" s="96" customFormat="1" ht="210" x14ac:dyDescent="0.25">
-      <c r="A19" s="95" t="s">
+    <row r="19" spans="1:7" s="54" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -5231,8 +5963,8 @@
       <c r="F19" s="51"/>
       <c r="G19" s="51"/>
     </row>
-    <row r="20" spans="1:7" s="96" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="95" t="s">
+    <row r="20" spans="1:7" s="54" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="53" t="s">
         <v>93</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -5250,30 +5982,30 @@
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
     </row>
-    <row r="21" spans="1:7" s="100" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="95" t="s">
+    <row r="21" spans="1:7" s="58" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="C21" s="99" t="s">
+      <c r="C21" s="57" t="s">
         <v>190</v>
       </c>
       <c r="D21" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="E21" s="99" t="s">
+      <c r="E21" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="F21" s="97"/>
-      <c r="G21" s="97"/>
-    </row>
-    <row r="22" spans="1:7" s="96" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="95" t="s">
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+    </row>
+    <row r="22" spans="1:7" s="54" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="56" t="s">
         <v>183</v>
       </c>
       <c r="C22" s="29" t="s">
@@ -5286,11 +6018,11 @@
       <c r="F22" s="51"/>
       <c r="G22" s="51"/>
     </row>
-    <row r="23" spans="1:7" s="96" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="95" t="s">
+    <row r="23" spans="1:7" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="56" t="s">
         <v>195</v>
       </c>
       <c r="C23" s="29" t="s">
@@ -5303,11 +6035,11 @@
       <c r="F23" s="51"/>
       <c r="G23" s="51"/>
     </row>
-    <row r="24" spans="1:7" s="96" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="95" t="s">
+    <row r="24" spans="1:7" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="56" t="s">
         <v>195</v>
       </c>
       <c r="C24" s="29" t="s">
@@ -5320,11 +6052,11 @@
       <c r="F24" s="51"/>
       <c r="G24" s="51"/>
     </row>
-    <row r="25" spans="1:7" s="96" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="95" t="s">
+    <row r="25" spans="1:7" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="56" t="s">
         <v>195</v>
       </c>
       <c r="C25" s="29" t="s">
@@ -5337,11 +6069,11 @@
       <c r="F25" s="51"/>
       <c r="G25" s="51"/>
     </row>
-    <row r="26" spans="1:7" s="96" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A26" s="95" t="s">
+    <row r="26" spans="1:7" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="98" t="s">
+      <c r="B26" s="56" t="s">
         <v>195</v>
       </c>
       <c r="C26" s="29" t="s">
@@ -5356,11 +6088,11 @@
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
     </row>
-    <row r="27" spans="1:7" s="96" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="95" t="s">
+    <row r="27" spans="1:7" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="56" t="s">
         <v>195</v>
       </c>
       <c r="C27" s="29" t="s">
@@ -5375,11 +6107,11 @@
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
     </row>
-    <row r="28" spans="1:7" s="96" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" s="95" t="s">
+    <row r="28" spans="1:7" s="54" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="56" t="s">
         <v>203</v>
       </c>
       <c r="C28" s="29" t="s">
@@ -5394,11 +6126,11 @@
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
     </row>
-    <row r="29" spans="1:7" s="96" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A29" s="95" t="s">
+    <row r="29" spans="1:7" s="54" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="56" t="s">
         <v>207</v>
       </c>
       <c r="C29" s="29" t="s">
@@ -5411,11 +6143,11 @@
       <c r="F29" s="51"/>
       <c r="G29" s="51"/>
     </row>
-    <row r="30" spans="1:7" s="96" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A30" s="95" t="s">
+    <row r="30" spans="1:7" s="54" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="56" t="s">
         <v>207</v>
       </c>
       <c r="C30" s="29" t="s">
@@ -5427,6 +6159,1289 @@
       <c r="E30" s="29"/>
       <c r="F30" s="51"/>
       <c r="G30" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G125"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
+    </row>
+    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="21">
+        <f>COUNTIF(F17:F31,"PASSED")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="88"/>
+      <c r="B7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="24">
+        <f>COUNTIF(F17:F31,"FAILED")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="91"/>
+      <c r="D8" s="43">
+        <f>SUM(C6,C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <f>SUM(D6,D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="44">
+        <f>COUNTIF(G17:G31,"PENDING")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="45">
+        <f>COUNTIF(F17:F31,"PENDING")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="95" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="45">
+        <f>COUNTIF(G17:G31,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="45">
+        <f>COUNTIF(F17:F31,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="45">
+        <f>COUNTIF(G17:G31,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="45">
+        <f>COUNTIF(F17:F31,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82">
+        <f>SUM(D8:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="82">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="16" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>242</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+    </row>
+    <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+    </row>
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+    </row>
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+    </row>
+    <row r="33" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+    </row>
+    <row r="34" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+    </row>
+    <row r="36" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+    </row>
+    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+    </row>
+    <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="101"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="101"/>
+      <c r="E40" s="101"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="101"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="101"/>
+      <c r="E41" s="101"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="101"/>
+      <c r="C42" s="101"/>
+      <c r="D42" s="101"/>
+      <c r="E42" s="101"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="101"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="101"/>
+      <c r="E43" s="101"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="101"/>
+      <c r="C44" s="101"/>
+      <c r="D44" s="101"/>
+      <c r="E44" s="101"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="101"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="101"/>
+      <c r="E45" s="101"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="101"/>
+      <c r="C46" s="101"/>
+      <c r="D46" s="101"/>
+      <c r="E46" s="101"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="101"/>
+      <c r="C47" s="101"/>
+      <c r="D47" s="101"/>
+      <c r="E47" s="101"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="101"/>
+      <c r="C48" s="101"/>
+      <c r="D48" s="101"/>
+      <c r="E48" s="101"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="101"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="101"/>
+      <c r="C50" s="101"/>
+      <c r="D50" s="101"/>
+      <c r="E50" s="101"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="101"/>
+      <c r="C51" s="101"/>
+      <c r="D51" s="101"/>
+      <c r="E51" s="101"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="101"/>
+      <c r="C52" s="101"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="101"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="101"/>
+      <c r="C53" s="101"/>
+      <c r="D53" s="101"/>
+      <c r="E53" s="101"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="101"/>
+      <c r="C54" s="101"/>
+      <c r="D54" s="101"/>
+      <c r="E54" s="101"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="101"/>
+      <c r="C55" s="101"/>
+      <c r="D55" s="101"/>
+      <c r="E55" s="101"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="101"/>
+      <c r="C56" s="101"/>
+      <c r="D56" s="101"/>
+      <c r="E56" s="101"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="101"/>
+      <c r="C57" s="101"/>
+      <c r="D57" s="101"/>
+      <c r="E57" s="101"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="101"/>
+      <c r="C58" s="101"/>
+      <c r="D58" s="101"/>
+      <c r="E58" s="101"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="101"/>
+      <c r="C59" s="101"/>
+      <c r="D59" s="101"/>
+      <c r="E59" s="101"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="101"/>
+      <c r="C60" s="101"/>
+      <c r="D60" s="101"/>
+      <c r="E60" s="101"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="101"/>
+      <c r="C61" s="101"/>
+      <c r="D61" s="101"/>
+      <c r="E61" s="101"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="101"/>
+      <c r="C62" s="101"/>
+      <c r="D62" s="101"/>
+      <c r="E62" s="101"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="101"/>
+      <c r="C63" s="101"/>
+      <c r="D63" s="101"/>
+      <c r="E63" s="101"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="101"/>
+      <c r="C64" s="101"/>
+      <c r="D64" s="101"/>
+      <c r="E64" s="101"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="101"/>
+      <c r="C65" s="101"/>
+      <c r="D65" s="101"/>
+      <c r="E65" s="101"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="101"/>
+      <c r="C66" s="101"/>
+      <c r="D66" s="101"/>
+      <c r="E66" s="101"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="101"/>
+      <c r="C67" s="101"/>
+      <c r="D67" s="101"/>
+      <c r="E67" s="101"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="101"/>
+      <c r="C68" s="101"/>
+      <c r="D68" s="101"/>
+      <c r="E68" s="101"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="101"/>
+      <c r="C69" s="101"/>
+      <c r="D69" s="101"/>
+      <c r="E69" s="101"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="101"/>
+      <c r="C70" s="101"/>
+      <c r="D70" s="101"/>
+      <c r="E70" s="101"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="101"/>
+      <c r="C71" s="101"/>
+      <c r="D71" s="101"/>
+      <c r="E71" s="101"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="101"/>
+      <c r="C72" s="101"/>
+      <c r="D72" s="101"/>
+      <c r="E72" s="101"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="101"/>
+      <c r="C73" s="101"/>
+      <c r="D73" s="101"/>
+      <c r="E73" s="101"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="101"/>
+      <c r="C74" s="101"/>
+      <c r="D74" s="101"/>
+      <c r="E74" s="101"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="101"/>
+      <c r="C75" s="101"/>
+      <c r="D75" s="101"/>
+      <c r="E75" s="101"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="101"/>
+      <c r="C76" s="101"/>
+      <c r="D76" s="101"/>
+      <c r="E76" s="101"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="101"/>
+      <c r="C77" s="101"/>
+      <c r="D77" s="101"/>
+      <c r="E77" s="101"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="101"/>
+      <c r="C78" s="101"/>
+      <c r="D78" s="101"/>
+      <c r="E78" s="101"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="101"/>
+      <c r="C79" s="101"/>
+      <c r="D79" s="101"/>
+      <c r="E79" s="101"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="101"/>
+      <c r="C80" s="101"/>
+      <c r="D80" s="101"/>
+      <c r="E80" s="101"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B81" s="101"/>
+      <c r="C81" s="101"/>
+      <c r="D81" s="101"/>
+      <c r="E81" s="101"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="101"/>
+      <c r="C82" s="101"/>
+      <c r="D82" s="101"/>
+      <c r="E82" s="101"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="101"/>
+      <c r="C83" s="101"/>
+      <c r="D83" s="101"/>
+      <c r="E83" s="101"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" s="101"/>
+      <c r="C84" s="101"/>
+      <c r="D84" s="101"/>
+      <c r="E84" s="101"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B85" s="101"/>
+      <c r="C85" s="101"/>
+      <c r="D85" s="101"/>
+      <c r="E85" s="101"/>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="101"/>
+      <c r="C86" s="101"/>
+      <c r="D86" s="101"/>
+      <c r="E86" s="101"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="101"/>
+      <c r="C87" s="101"/>
+      <c r="D87" s="101"/>
+      <c r="E87" s="101"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="101"/>
+      <c r="C88" s="101"/>
+      <c r="D88" s="101"/>
+      <c r="E88" s="101"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="101"/>
+      <c r="C89" s="101"/>
+      <c r="D89" s="101"/>
+      <c r="E89" s="101"/>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="101"/>
+      <c r="C90" s="101"/>
+      <c r="D90" s="101"/>
+      <c r="E90" s="101"/>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="101"/>
+      <c r="C91" s="101"/>
+      <c r="D91" s="101"/>
+      <c r="E91" s="101"/>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="101"/>
+      <c r="C92" s="101"/>
+      <c r="D92" s="101"/>
+      <c r="E92" s="101"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="101"/>
+      <c r="C93" s="101"/>
+      <c r="D93" s="101"/>
+      <c r="E93" s="101"/>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="101"/>
+      <c r="C94" s="101"/>
+      <c r="D94" s="101"/>
+      <c r="E94" s="101"/>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="101"/>
+      <c r="C95" s="101"/>
+      <c r="D95" s="101"/>
+      <c r="E95" s="101"/>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="101"/>
+      <c r="C96" s="101"/>
+      <c r="D96" s="101"/>
+      <c r="E96" s="101"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="101"/>
+      <c r="C97" s="101"/>
+      <c r="D97" s="101"/>
+      <c r="E97" s="101"/>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="101"/>
+      <c r="C98" s="101"/>
+      <c r="D98" s="101"/>
+      <c r="E98" s="101"/>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="101"/>
+      <c r="C99" s="101"/>
+      <c r="D99" s="101"/>
+      <c r="E99" s="101"/>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="101"/>
+      <c r="C100" s="101"/>
+      <c r="D100" s="101"/>
+      <c r="E100" s="101"/>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="101"/>
+      <c r="C101" s="101"/>
+      <c r="D101" s="101"/>
+      <c r="E101" s="101"/>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="101"/>
+      <c r="C102" s="101"/>
+      <c r="D102" s="101"/>
+      <c r="E102" s="101"/>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="101"/>
+      <c r="C103" s="101"/>
+      <c r="D103" s="101"/>
+      <c r="E103" s="101"/>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="101"/>
+      <c r="C104" s="101"/>
+      <c r="D104" s="101"/>
+      <c r="E104" s="101"/>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="101"/>
+      <c r="C105" s="101"/>
+      <c r="D105" s="101"/>
+      <c r="E105" s="101"/>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="101"/>
+      <c r="C106" s="101"/>
+      <c r="D106" s="101"/>
+      <c r="E106" s="101"/>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="101"/>
+      <c r="C107" s="101"/>
+      <c r="D107" s="101"/>
+      <c r="E107" s="101"/>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="101"/>
+      <c r="C108" s="101"/>
+      <c r="D108" s="101"/>
+      <c r="E108" s="101"/>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="101"/>
+      <c r="C109" s="101"/>
+      <c r="D109" s="101"/>
+      <c r="E109" s="101"/>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="101"/>
+      <c r="C110" s="101"/>
+      <c r="D110" s="101"/>
+      <c r="E110" s="101"/>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="101"/>
+      <c r="C111" s="101"/>
+      <c r="D111" s="101"/>
+      <c r="E111" s="101"/>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="101"/>
+      <c r="C112" s="101"/>
+      <c r="D112" s="101"/>
+      <c r="E112" s="101"/>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" s="101"/>
+      <c r="C113" s="101"/>
+      <c r="D113" s="101"/>
+      <c r="E113" s="101"/>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="101"/>
+      <c r="C114" s="101"/>
+      <c r="D114" s="101"/>
+      <c r="E114" s="101"/>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115" s="101"/>
+      <c r="C115" s="101"/>
+      <c r="D115" s="101"/>
+      <c r="E115" s="101"/>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="101"/>
+      <c r="C116" s="101"/>
+      <c r="D116" s="101"/>
+      <c r="E116" s="101"/>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="101"/>
+      <c r="C117" s="101"/>
+      <c r="D117" s="101"/>
+      <c r="E117" s="101"/>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="101"/>
+      <c r="C118" s="101"/>
+      <c r="D118" s="101"/>
+      <c r="E118" s="101"/>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119" s="101"/>
+      <c r="C119" s="101"/>
+      <c r="D119" s="101"/>
+      <c r="E119" s="101"/>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120" s="101"/>
+      <c r="C120" s="101"/>
+      <c r="D120" s="101"/>
+      <c r="E120" s="101"/>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121" s="101"/>
+      <c r="C121" s="101"/>
+      <c r="D121" s="101"/>
+      <c r="E121" s="101"/>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B122" s="101"/>
+      <c r="C122" s="101"/>
+      <c r="D122" s="101"/>
+      <c r="E122" s="101"/>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B123" s="101"/>
+      <c r="C123" s="101"/>
+      <c r="D123" s="101"/>
+      <c r="E123" s="101"/>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="101"/>
+      <c r="C124" s="101"/>
+      <c r="D124" s="101"/>
+      <c r="E124" s="101"/>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="101"/>
+      <c r="C125" s="101"/>
+      <c r="D125" s="101"/>
+      <c r="E125" s="101"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
+    </row>
+    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="21">
+        <f>COUNTIF(F17:F31,"PASSED")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="88"/>
+      <c r="B7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="24">
+        <f>COUNTIF(F17:F31,"FAILED")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="91"/>
+      <c r="D8" s="43">
+        <f>SUM(C6,C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <f>SUM(D6,D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="44">
+        <f>COUNTIF(G17:G31,"PENDING")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="45">
+        <f>COUNTIF(F17:F31,"PENDING")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="95" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="45">
+        <f>COUNTIF(G17:G31,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="45">
+        <f>COUNTIF(F17:F31,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="45">
+        <f>COUNTIF(G17:G31,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="45">
+        <f>COUNTIF(F17:F31,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82">
+        <f>SUM(D8:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="82">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="16" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Added test case for checkout page in Ninja_Isango_Test_Cases.xlsx
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="685" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="280">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1083,16 +1083,130 @@
     <t>Checkout</t>
   </si>
   <si>
+    <t>Verify application display Checkout page.</t>
+  </si>
+  <si>
     <t>1. Launch Ninja specific URL.
 2. User is on Home Page
 3. Click on product that have options.
 4. User is on product detail page.
 5. Enter valid information and click on Check availability button
 6. User is on availability page and click on add to cart.
-7. User is on Cart page and click on secure checkout</t>
-  </si>
-  <si>
-    <t>Verify application display Checkout page.</t>
+7. User is on Cart page and click on secure checkout
+8. User is on Checkout page.</t>
+  </si>
+  <si>
+    <t>1. User is on Cart page and click on secure checkout
+2. User is on Checkout page.</t>
+  </si>
+  <si>
+    <t>Verify application display below mentioned items in header:
+1. Text "A part of TUI Travel PLC group of companies”
+2. About US
+3. WebSite Logo
+4. Contact Number
+5. Lowest Price Guarantee
+6. Flexible Cancellation
+7. Local Expertise
+8. Happy Customers
+9. Read reviews</t>
+  </si>
+  <si>
+    <t>Verify Application display below mentioned tabs:
+1. Your details (Highlighted)
+2. Payment
+3. Confirm</t>
+  </si>
+  <si>
+    <t>Verify aaplication displays below mentioned information in footer:
+1. Your payment protected by (Logo)
+2. About Us 
+3. Customer Care 
+4. Terms &amp; Conditions 
+5. Isango logo
+6. Social Media Icons.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application navigate user to appropriate page when user click on any link display </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify application display below mentioned information and items for all product added:
+1. Product Name
+2. Product Price
+3. Location
+4. Start date
+5. Availability
+6. Lead Traveller Name (First Name and Last Name)
+7. Meeting point
+8. Special request 
+</t>
+  </si>
+  <si>
+    <t>Application display these informtion with eacch product display on checkout page.</t>
+  </si>
+  <si>
+    <t>Verify application displays below mentioned information in right pane:
+1. Booking Summary
+2. Call us 24/7</t>
+  </si>
+  <si>
+    <t>Verify below mentioned items display for each product under Booking Summary:
+1. Product Name
+2. Product Price
+3. Cancellation policy
+4. Show details</t>
+  </si>
+  <si>
+    <t>1. User is on Cart page and click on secure checkout
+2. User is on Checkout page.
+3. Click on "Cancellation policy" display under Booking summery</t>
+  </si>
+  <si>
+    <t>Verify application display pane with cross button to close the same, when user click on link "Cancellation policy" display under Booking Summery</t>
+  </si>
+  <si>
+    <t>Verify application display below mentioned information when user click on "Show details" display under booking summery:
+1. Tour Date
+2. Number of adults</t>
+  </si>
+  <si>
+    <t>Application does same behaviour for all link "Cancellation policy" display under Booking Summery</t>
+  </si>
+  <si>
+    <t>Application does same behaviour for all link "Show Details" display under Booking Summery</t>
+  </si>
+  <si>
+    <t>1. User is on Cart page and click on secure checkout
+2. User is on Checkout page.
+3. Click on "Show Dteails" display under Booking summery</t>
+  </si>
+  <si>
+    <t>Verify application display total price to pay at the end of section booking summery.</t>
+  </si>
+  <si>
+    <t>Verify application display multisave when user added more than one item in cart and total pay price calculated accordigly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on Cart page and click on secure checkout
+2. User is on Checkout page.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on Cart page with more than 2 products and click on secure checkout.
+2. User is on Checkout page.
+</t>
+  </si>
+  <si>
+    <t>Verify application display message when user left name fields blank.
+1. Please enter the first name
+2. Please enter the Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on Cart page with more than 2 products and click on secure checkout.
+2. User is on Checkout page.
+3. Left name field blank
+4. Click on Proceed to payment
+</t>
   </si>
 </sst>
 </file>
@@ -3726,7 +3840,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C28"/>
+      <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,7 +4100,10 @@
       <c r="A28" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="B28" s="59"/>
+      <c r="B28" s="59">
+        <f>COUNTIF(Checkout!A17:A70,"*")</f>
+        <v>12</v>
+      </c>
       <c r="C28" s="60"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4009,7 +4126,7 @@
       </c>
       <c r="B31" s="71">
         <f>SUM(B23:B30)</f>
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C31" s="72"/>
     </row>
@@ -4618,7 +4735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -7254,17 +7371,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -7433,15 +7550,431 @@
         <v>90</v>
       </c>
       <c r="B17" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>257</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>258</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="D21" s="50"/>
+      <c r="E21" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D24" s="50"/>
+      <c r="E24" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="50"/>
+      <c r="E25" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>274</v>
+      </c>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+    </row>
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>275</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="30"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="30"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="30"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="30"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="30"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="30"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="30"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="30"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="30"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="28"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="30"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="30"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="30"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="30"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="28"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="30"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="30"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="30"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="30"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="28"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="30"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="30"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="30"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="30"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Update test cases in Ninja_Isango_Test_Cases.xlsx
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="685" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="685" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="282">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1206,6 +1206,14 @@
 2. User is on Checkout page.
 3. Left name field blank
 4. Click on Proceed to payment
+</t>
+  </si>
+  <si>
+    <t>Verify application display cart opage when user click on "Back to Cart" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on Cart page with more than 2 products and click on secure checkout.
+2. User is on Checkout page.
 </t>
   </si>
 </sst>
@@ -3839,7 +3847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
@@ -4102,7 +4110,7 @@
       </c>
       <c r="B28" s="59">
         <f>COUNTIF(Checkout!A17:A70,"*")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="60"/>
     </row>
@@ -4126,7 +4134,7 @@
       </c>
       <c r="B31" s="71">
         <f>SUM(B23:B30)</f>
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C31" s="72"/>
     </row>
@@ -4180,7 +4188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -5390,7 +5398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -7373,8 +7381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7733,10 +7741,16 @@
       <c r="F28" s="28"/>
       <c r="G28" s="28"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>280</v>
+      </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>

</xml_diff>

<commit_message>
Updated Mail and Voucher Business Rules.jpg Updated detail description documents.
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="685" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="725" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Availability Page" sheetId="7" r:id="rId5"/>
     <sheet name="Cart Page" sheetId="8" r:id="rId6"/>
     <sheet name="Checkout" sheetId="9" r:id="rId7"/>
+    <sheet name="Payment Page" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="290">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1215,6 +1216,51 @@
     <t xml:space="preserve">1. User is on Cart page with more than 2 products and click on secure checkout.
 2. User is on Checkout page.
 </t>
+  </si>
+  <si>
+    <t>Verify application displays payment page when user click on "Proceed to payment" button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on Cart page with more than 2 products and click on secure checkout.
+2. User is on Checkout page.
+3. Enter information.
+4. Click on "Proceed to payment" button.
+</t>
+  </si>
+  <si>
+    <t>Verify application display home page when user click on website logo display on topleft corner.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User is on Cart page with more than 2 products and click on secure checkout.
+2. User is on Checkout page.
+3. Click on website logo.
+</t>
+  </si>
+  <si>
+    <t>1. Launch Ninja specific URL.
+2. User is on Home Page
+3. Click on product that have options.
+4. User is on product detail page.
+5. Enter valid information and click on Check availability button
+6. User is on availability page and click on add to cart.
+7. User is on Cart page and click on secure checkout
+8. User is on Checkout page.
+9. Enter information.
+10. Click on "Proceed to payment" button.</t>
+  </si>
+  <si>
+    <t>1. User is on payment page.</t>
+  </si>
+  <si>
+    <t>Verify Application display below mentioned tabs:
+1. Your details 
+2. Payment (Highlighted)
+3. Confirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify application display below mentioned areas on payment page:
+1. Contact Information 
+2. </t>
   </si>
 </sst>
 </file>
@@ -3582,6 +3628,251 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="66675"/>
+          <a:ext cx="1781175" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000"/>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3847,7 +4138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
@@ -4110,7 +4401,7 @@
       </c>
       <c r="B28" s="59">
         <f>COUNTIF(Checkout!A17:A70,"*")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C28" s="60"/>
     </row>
@@ -4118,7 +4409,10 @@
       <c r="A29" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B29" s="59"/>
+      <c r="B29" s="59">
+        <f>COUNTIF('Payment Page'!A17:A70,"*")</f>
+        <v>10</v>
+      </c>
       <c r="C29" s="60"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4134,7 +4428,7 @@
       </c>
       <c r="B31" s="71">
         <f>SUM(B23:B30)</f>
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C31" s="72"/>
     </row>
@@ -5398,7 +5692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -7381,8 +7675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A29"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7756,19 +8050,31 @@
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+    <row r="30" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>282</v>
+      </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+    <row r="31" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>284</v>
+      </c>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
@@ -7777,7 +8083,7 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
@@ -7786,7 +8092,7 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
@@ -7795,7 +8101,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
       <c r="F34" s="28"/>
@@ -7804,7 +8110,7 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
@@ -7813,7 +8119,7 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
       <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
       <c r="F36" s="28"/>
@@ -7822,7 +8128,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
       <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
+      <c r="C37" s="29"/>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
       <c r="F37" s="28"/>
@@ -8006,4 +8312,340 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73"/>
+      <c r="B1" s="74"/>
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
+    </row>
+    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75"/>
+      <c r="B3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+    </row>
+    <row r="5" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="21">
+        <f>COUNTIF(F17:F31,"PASSED")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="88"/>
+      <c r="B7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="24">
+        <f>COUNTIF(F17:F31,"FAILED")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="89"/>
+      <c r="B8" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="91"/>
+      <c r="D8" s="43">
+        <f>SUM(C6,C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="49">
+        <f>SUM(D6,D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="93"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="44">
+        <f>COUNTIF(G17:G31,"PENDING")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="45">
+        <f>COUNTIF(F17:F31,"PENDING")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="95" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="96"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="45">
+        <f>COUNTIF(G17:G31,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="45">
+        <f>COUNTIF(F17:F31,"IN PROGRESS")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="45">
+        <f>COUNTIF(G17:G31,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="45">
+        <f>COUNTIF(F17:F31,"BLOCKED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="82">
+        <f>SUM(D8:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="82">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+    </row>
+    <row r="14" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="16" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:B4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Cover Page'!$A$38:$A$46</xm:f>
+          </x14:formula1>
+          <xm:sqref>F17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test cases for payment page
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="304">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1258,9 +1258,87 @@
 3. Confirm</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify application display below mentioned areas on payment page:
+    <t>Verify application display below mentioned areas on payment page:
 1. Contact Information 
-2. </t>
+2. Secure Card Payment
+3. Billing Address</t>
+  </si>
+  <si>
+    <t>Application display below mentioned fields under Contact Information section:
+1. Email address
+2. Confirm email address
+3. Phone</t>
+  </si>
+  <si>
+    <t>Application display below mentioned fields under Secure Card Payment section:
+1. Card type*
+2. Card Number*
+3. Cardholder name*
+4. Expiry date*
+5. Security code*
+6. What is this?</t>
+  </si>
+  <si>
+    <t>Application display below mentioned fields under  Billing Address section:
+1. Address (Line1)*
+2. Address (Line 2) 
+3. City*
+4. Country/State 
+5. Post code/ Zip code*
+6. Country*
+7. Terms &amp; Conditions</t>
+  </si>
+  <si>
+    <t>Verify applicationn displays "Confirm and Pay" button</t>
+  </si>
+  <si>
+    <t>1. User is on payment page.
+2. Click on "Cancellation policy"</t>
+  </si>
+  <si>
+    <t>1. User is on payment page.
+2. Click on "Show details"</t>
+  </si>
+  <si>
+    <t>Verify error messages when user left any reletive field blank under Contact Information  and click on Confirm and Pay button:
+1. Please enter your email address
+2. Please enter your email address
+3. Please enter phone number</t>
+  </si>
+  <si>
+    <t>Verify error messages when user left any reletive field blank under Secure Card Payment  and click on Confirm and Pay button:
+1. Please enter the numeric card number
+2. Please enter the name
+3. Please enter the security code</t>
+  </si>
+  <si>
+    <t>Verify application display checkout page when user click on Your Details tab display under header.</t>
+  </si>
+  <si>
+    <t>1. User is on payment page.
+2. Left fields blank under Contact Information
+3. Click on Confirm and Pay button.</t>
+  </si>
+  <si>
+    <t>1. User is on payment page.
+2. Left fields blank under Secure Card Payment
+3. Click on Confirm and Pay button.</t>
+  </si>
+  <si>
+    <t>Verify error messages when user left any reletive field blank under  Billing Address  and click on Confirm and Pay button:
+1. Please enter the Address1
+2. Please enter the city
+3. Please enter the Post code/Zip code
+4. Please enter Terms &amp; conditions to proceed</t>
+  </si>
+  <si>
+    <t>1. User is on payment page.
+2. Left fields blank under Billing Address
+3. Click on Confirm and Pay button.</t>
+  </si>
+  <si>
+    <t>1. User is on payment page.
+2. Click on Your Details tab.</t>
   </si>
 </sst>
 </file>
@@ -4138,7 +4216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
@@ -4410,8 +4488,8 @@
         <v>63</v>
       </c>
       <c r="B29" s="59">
-        <f>COUNTIF('Payment Page'!A17:A70,"*")</f>
-        <v>10</v>
+        <f>COUNTIF('Payment Page'!A17:A69,"*")</f>
+        <v>19</v>
       </c>
       <c r="C29" s="60"/>
     </row>
@@ -4428,7 +4506,7 @@
       </c>
       <c r="B31" s="71">
         <f>SUM(B23:B30)</f>
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C31" s="72"/>
     </row>
@@ -7675,8 +7753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8316,10 +8394,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8551,11 +8629,13 @@
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
     </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="29" t="s">
+        <v>287</v>
+      </c>
       <c r="C21" s="29" t="s">
         <v>289</v>
       </c>
@@ -8564,60 +8644,215 @@
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>290</v>
+      </c>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
+      <c r="B23" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>291</v>
+      </c>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
+      <c r="B24" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>292</v>
+      </c>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
+      <c r="B25" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>293</v>
+      </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
+      <c r="B26" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>266</v>
+      </c>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
+    </row>
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="C29" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="50" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+    </row>
+    <row r="32" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>296</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+    </row>
+    <row r="33" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="C33" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+    </row>
+    <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="C34" s="50" t="s">
+        <v>301</v>
+      </c>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="C35" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -8642,7 +8877,7 @@
           <x14:formula1>
             <xm:f>'Cover Page'!$A$38:$A$46</xm:f>
           </x14:formula1>
-          <xm:sqref>F17</xm:sqref>
+          <xm:sqref>F17:F35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Updated test cases in Ninja_Isango_Test_Cases.xlsx
</commit_message>
<xml_diff>
--- a/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
+++ b/Updated TestCases/Ninja/Regression TestCases/Ninja_Isango_Test_Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="725" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="339">
   <si>
     <t>Project Name:</t>
   </si>
@@ -1468,23 +1468,20 @@
 3. Open PDF voucher</t>
   </si>
   <si>
-    <t>Application dispalys ninja website logo on topleft corner.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application display Isango logo on top right corner </t>
-  </si>
-  <si>
-    <t>Application display booking refrence number</t>
-  </si>
-  <si>
-    <t>Application display below mentioned sections in PDF voucher
+    <t xml:space="preserve">Verify application display Isango logo on top right corner </t>
+  </si>
+  <si>
+    <t>Verify application display booking refrence number</t>
+  </si>
+  <si>
+    <t>Verify application display below mentioned sections in PDF voucher
 1. Booking Information
 2. Tour Schedule
 3. Contact Details
 4. Payment Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">Application displays below mentioned fields under booking section:
+    <t xml:space="preserve">Verify application displays below mentioned fields under booking section:
 1. Lead Traveller 
 2. Tour Booked 
 3. Option Name 
@@ -1495,7 +1492,7 @@
 8. Special Request </t>
   </si>
   <si>
-    <t xml:space="preserve">Application displays below mentioned fields under Tour Schedule:
+    <t xml:space="preserve">Verify application displays below mentioned fields under Tour Schedule:
 1. Meeting Point 
 2. Ending Point 
 3. Start Time 
@@ -1503,17 +1500,23 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Application displays below mentioned fields under Contact Details:
+    <t xml:space="preserve">Verify application displays below mentioned fields under Contact Details:
 1. Need further assistance or bookings
 2. Email </t>
   </si>
   <si>
-    <t xml:space="preserve">Application displays below mentioned fields under Payment Summary:
+    <t xml:space="preserve">Verify application displays below mentioned fields under Payment Summary:
 1. Product Name 
 2. Price
 3. Total Booking Amount 
 4. Total Charged Amount 
 5.  To be Charged on Confirmation ofPending Booking Requests </t>
+  </si>
+  <si>
+    <t>Verify application dispalys ninja website logo on topleft corner.</t>
+  </si>
+  <si>
+    <t>Verify application displays same information as entered by user while making booking for products.</t>
   </si>
 </sst>
 </file>
@@ -1612,7 +1615,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -2075,23 +2078,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2398,9 +2390,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4650,7 +4639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B31" sqref="B31:C31"/>
     </sheetView>
   </sheetViews>
@@ -4932,8 +4921,8 @@
         <v>64</v>
       </c>
       <c r="B30" s="60">
-        <f>COUNTIF('Confirmation Page'!A17:A69,"*")</f>
-        <v>23</v>
+        <f>COUNTIF('Confirmation Page'!A17:A59,"*")</f>
+        <v>24</v>
       </c>
       <c r="C30" s="61"/>
     </row>
@@ -4943,7 +4932,7 @@
       </c>
       <c r="B31" s="72">
         <f>SUM(B23:B30)</f>
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C31" s="73"/>
     </row>
@@ -7116,8 +7105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8190,8 +8179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C27"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9399,10 +9388,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9807,7 +9796,7 @@
         <v>329</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
@@ -9822,7 +9811,7 @@
         <v>329</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
@@ -9837,7 +9826,7 @@
         <v>329</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="28"/>
@@ -9852,7 +9841,7 @@
         <v>329</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D35" s="28"/>
       <c r="E35" s="28"/>
@@ -9867,7 +9856,7 @@
         <v>329</v>
       </c>
       <c r="C36" s="52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="28"/>
@@ -9882,7 +9871,7 @@
         <v>329</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D37" s="28"/>
       <c r="E37" s="28"/>
@@ -9897,7 +9886,7 @@
         <v>329</v>
       </c>
       <c r="C38" s="52" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D38" s="28"/>
       <c r="E38" s="28"/>
@@ -9912,36 +9901,27 @@
         <v>329</v>
       </c>
       <c r="C39" s="52" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D39" s="28"/>
       <c r="E39" s="28"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="102"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="102"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="102"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="102"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="102"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="102"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="102"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="102"/>
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>338</v>
+      </c>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>